<commit_message>
Writing an Excel File
</commit_message>
<xml_diff>
--- a/Laboratoare paradigme/Laborator8/src/Output.xlsx
+++ b/Laboratoare paradigme/Laborator8/src/Output.xlsx
@@ -12,7 +12,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Vasile</t>
+  </si>
+  <si>
+    <t>Ionescu</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Acu</t>
+  </si>
+  <si>
+    <t>Nicu</t>
+  </si>
+  <si>
+    <t>Radu</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,12 +80,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="n" s="0">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>41.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>